<commit_message>
Hong dang lam tinh nang bat ma mau trung, ko pull
</commit_message>
<xml_diff>
--- a/DataProcessing/vd-minh-hoa.xlsx
+++ b/DataProcessing/vd-minh-hoa.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nam\Desktop\s\Project1\DataProcessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuanh\Desktop\Project1\DataProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>A</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
   </si>
   <si>
     <t>G</t>
@@ -366,15 +363,15 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -391,13 +388,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>42680</v>
       </c>
@@ -405,12 +402,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>42681</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>42682</v>
       </c>
@@ -418,17 +418,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>42683</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>42684</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>42685</v>
       </c>
@@ -436,7 +439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>42686</v>
       </c>

</xml_diff>

<commit_message>
Hong update xoa, doi ten dau trung cho nhom 2 mau
</commit_message>
<xml_diff>
--- a/DataProcessing/vd-minh-hoa.xlsx
+++ b/DataProcessing/vd-minh-hoa.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuanh\Desktop\Project1\DataProcessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuanh_000\Desktop\Project1\DataProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>A</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -360,18 +363,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -393,16 +396,31 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42680</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42681</v>
       </c>
@@ -410,36 +428,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42682</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42683</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42684</v>
       </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
       <c r="G6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42685</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42686</v>
       </c>

</xml_diff>

<commit_message>
Hong fix doi ten
</commit_message>
<xml_diff>
--- a/DataProcessing/vd-minh-hoa.xlsx
+++ b/DataProcessing/vd-minh-hoa.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuanh_000\Desktop\Project1\DataProcessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuanh\Desktop\Project1\DataProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>A</t>
   </si>
@@ -41,10 +41,7 @@
     <t>E</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>F</t>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -363,18 +360,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -396,14 +393,8 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>42680</v>
       </c>
@@ -413,14 +404,8 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>42681</v>
       </c>
@@ -428,29 +413,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>42682</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>42683</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>42684</v>
       </c>
@@ -461,18 +440,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>42685</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>42686</v>
       </c>

</xml_diff>

<commit_message>
Hong update gop 1 mau trung
</commit_message>
<xml_diff>
--- a/DataProcessing/vd-minh-hoa.xlsx
+++ b/DataProcessing/vd-minh-hoa.xlsx
@@ -363,7 +363,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,9 +417,6 @@
       <c r="A4" s="1">
         <v>42682</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -451,9 +448,6 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>42686</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hong update tinh chinh dau vao
</commit_message>
<xml_diff>
--- a/DataProcessing/vd-minh-hoa.xlsx
+++ b/DataProcessing/vd-minh-hoa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>A</t>
   </si>
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -371,7 +371,7 @@
     <col min="1" max="1" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -393,8 +393,17 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>42680</v>
       </c>
@@ -405,7 +414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>42681</v>
       </c>
@@ -413,12 +422,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>42682</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>42683</v>
       </c>
@@ -426,7 +438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>42684</v>
       </c>
@@ -437,7 +449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>42685</v>
       </c>
@@ -445,9 +457,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>42686</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>